<commit_message>
what is wrong with curvefit
</commit_message>
<xml_diff>
--- a/Pendulum/F3_Fadenpendel.xlsx
+++ b/Pendulum/F3_Fadenpendel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huyenanh/git_repos/MB14_Classical_mechanics/Pendulum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A06EC6-A234-0040-94DA-903459A2BE42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC8136A-D3AE-B34F-AECA-C3AB4DBD82B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19380" yWindow="3640" windowWidth="28080" windowHeight="17120" activeTab="2" xr2:uid="{0C87622E-8A3E-9447-883B-E874DD3727AC}"/>
+    <workbookView xWindow="1700" yWindow="760" windowWidth="16560" windowHeight="18880" activeTab="2" xr2:uid="{0C87622E-8A3E-9447-883B-E874DD3727AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Durchführung" sheetId="3" r:id="rId1"/>
@@ -3894,8 +3894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1BFBAD4-91D6-1248-A7D7-448FD96D1BCC}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4359,14 +4359,14 @@
     </row>
     <row r="30" spans="1:11" ht="22" customHeight="1" thickBot="1">
       <c r="A30" s="38">
-        <v>2.25</v>
+        <v>3.25</v>
       </c>
       <c r="B30" s="43">
         <f>SQRT((B17)^2 + D17^2)</f>
         <v>0.70000071428534982</v>
       </c>
       <c r="C30">
-        <v>96.419999999999987</v>
+        <v>20.329999999999998</v>
       </c>
       <c r="D30" s="33">
         <f>E30-0.1</f>
@@ -4387,14 +4387,14 @@
     </row>
     <row r="31" spans="1:11" ht="22" customHeight="1">
       <c r="A31" s="38">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B31" s="33">
         <f>SQRT((B18)^2 + D18^2)</f>
         <v>1E-3</v>
       </c>
       <c r="C31">
-        <v>90.8</v>
+        <v>19.91</v>
       </c>
       <c r="D31" s="33">
         <f t="shared" ref="D31:D39" si="1">E31-0.1</f>
@@ -4406,14 +4406,14 @@
     </row>
     <row r="32" spans="1:11" ht="22" customHeight="1">
       <c r="A32" s="38">
-        <v>1.75</v>
+        <v>2.75</v>
       </c>
       <c r="B32" s="33">
         <f t="shared" ref="B32:B38" si="2">SQRT((B19)^2 + D19^2)</f>
         <v>1E-3</v>
       </c>
       <c r="C32">
-        <v>80.599999999999994</v>
+        <v>19.5</v>
       </c>
       <c r="D32" s="33">
         <f t="shared" si="1"/>
@@ -4425,14 +4425,14 @@
     </row>
     <row r="33" spans="1:8" ht="22" customHeight="1">
       <c r="A33" s="38">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="B33" s="33">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
       <c r="C33">
-        <v>70.5</v>
+        <v>19.14</v>
       </c>
       <c r="D33" s="33">
         <f t="shared" si="1"/>
@@ -4447,14 +4447,14 @@
     </row>
     <row r="34" spans="1:8" ht="22" customHeight="1">
       <c r="A34" s="38">
-        <v>1.25</v>
+        <v>2.25</v>
       </c>
       <c r="B34" s="33">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
       <c r="C34">
-        <v>60.4</v>
+        <v>18.72</v>
       </c>
       <c r="D34" s="33">
         <f t="shared" si="1"/>
@@ -4469,14 +4469,14 @@
     </row>
     <row r="35" spans="1:8" ht="22" customHeight="1">
       <c r="A35" s="38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B35" s="33">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
       <c r="C35">
-        <v>50.6</v>
+        <v>18.3</v>
       </c>
       <c r="D35" s="33">
         <f t="shared" si="1"/>
@@ -4488,14 +4488,14 @@
     </row>
     <row r="36" spans="1:8" ht="22" customHeight="1">
       <c r="A36" s="38">
-        <v>0.75</v>
+        <v>1.75</v>
       </c>
       <c r="B36" s="33">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
       <c r="C36">
-        <v>40.299999999999997</v>
+        <v>17.77</v>
       </c>
       <c r="D36" s="33">
         <f t="shared" si="1"/>
@@ -4507,14 +4507,14 @@
     </row>
     <row r="37" spans="1:8" ht="22" customHeight="1">
       <c r="A37" s="38">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="B37" s="33">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
       <c r="C37">
-        <v>30.2</v>
+        <v>17.350000000000001</v>
       </c>
       <c r="D37" s="33">
         <f t="shared" si="1"/>
@@ -4526,14 +4526,14 @@
     </row>
     <row r="38" spans="1:8" ht="22" customHeight="1">
       <c r="A38" s="38">
-        <v>0.25</v>
+        <v>1.25</v>
       </c>
       <c r="B38" s="33">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
       <c r="C38">
-        <v>20.3</v>
+        <v>16.79</v>
       </c>
       <c r="D38" s="33">
         <f t="shared" si="1"/>
@@ -4545,14 +4545,14 @@
     </row>
     <row r="39" spans="1:8" ht="22" customHeight="1" thickBot="1">
       <c r="A39" s="40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B39" s="44">
         <f>SQRT((B26)^2 + D26^2)</f>
         <v>0.50000099999899994</v>
       </c>
       <c r="C39" s="41">
-        <v>0</v>
+        <v>16.46</v>
       </c>
       <c r="D39" s="34">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
square period and r is missing"
exit()
"
</commit_message>
<xml_diff>
--- a/Pendulum/F3_Fadenpendel.xlsx
+++ b/Pendulum/F3_Fadenpendel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huyenanh/git_repos/MB14_Classical_mechanics/Pendulum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A6823A-6C9A-D548-AF39-8E69EE5174F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D419F713-C4D3-3C4E-928D-F67FC65B3BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="760" windowWidth="28300" windowHeight="18880" activeTab="1" xr2:uid="{0C87622E-8A3E-9447-883B-E874DD3727AC}"/>
   </bookViews>
@@ -793,7 +793,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="16">
     <font>
@@ -972,7 +972,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -987,60 +987,7 @@
   </cellStyles>
   <dxfs count="38">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.000"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.000"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.000"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri-Light"/>
-        <scheme val="none"/>
-      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1083,6 +1030,78 @@
         <name val="Calibri-Light"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri-Light"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1193,25 +1212,6 @@
         <name val="Calibri-Light"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -2579,28 +2579,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{74E82EF0-C58F-BB4B-8EBC-87C952B8B3B9}" name="Table3" displayName="Table3" ref="B3:C13" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{74E82EF0-C58F-BB4B-8EBC-87C952B8B3B9}" name="Table3" displayName="Table3" ref="B3:C13" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
   <autoFilter ref="B3:C13" xr:uid="{74E82EF0-C58F-BB4B-8EBC-87C952B8B3B9}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{8346DB69-F8D0-374E-98BD-0B1E887C0365}" name="T(Nullpunkt) in s" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{04C0E93E-E90D-E94D-80A9-BA066B3C0889}" name="T(Umkehrpunkt) in s" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{8346DB69-F8D0-374E-98BD-0B1E887C0365}" name="T(Nullpunkt) in s" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{04C0E93E-E90D-E94D-80A9-BA066B3C0889}" name="T(Umkehrpunkt) in s" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{270A50D9-6F60-2545-AF66-7BABDD5BAB15}" name="Table4" displayName="Table4" ref="B37:C49" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{270A50D9-6F60-2545-AF66-7BABDD5BAB15}" name="Table4" displayName="Table4" ref="B37:C49" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="B37:C49" xr:uid="{270A50D9-6F60-2545-AF66-7BABDD5BAB15}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{EC12AF92-6AA2-A148-9B1E-938F14924331}" name="li,ges in m" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{6A5DF10D-FF45-B14C-A13B-2628E98996BF}" name="∆liEG in mm" dataDxfId="24">
+    <tableColumn id="1" xr3:uid="{EC12AF92-6AA2-A148-9B1E-938F14924331}" name="li,ges in m" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{6A5DF10D-FF45-B14C-A13B-2628E98996BF}" name="∆liEG in mm" dataDxfId="30">
       <calculatedColumnFormula>SQRT((#REF!)^2 + D21^2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2609,21 +2609,21 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{ED8BB0E8-9CA0-AB4C-8485-913DC6849F9B}" name="Table5" displayName="Table5" ref="O44:P45" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{ED8BB0E8-9CA0-AB4C-8485-913DC6849F9B}" name="Table5" displayName="Table5" ref="O44:P45" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="O44:P45" xr:uid="{ED8BB0E8-9CA0-AB4C-8485-913DC6849F9B}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{E53F5F5C-3534-0B48-931B-7E4E85D8B3E8}" name="a" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{CA60A8C6-6B33-7141-9408-E626FCFBE907}" name="b" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{E53F5F5C-3534-0B48-931B-7E4E85D8B3E8}" name="a" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{CA60A8C6-6B33-7141-9408-E626FCFBE907}" name="b" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium24" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8AF7BB84-E4B4-AE4E-877F-000F781757C1}" name="Table1" displayName="Table1" ref="B20:E32" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8AF7BB84-E4B4-AE4E-877F-000F781757C1}" name="Table1" displayName="Table1" ref="B20:E32" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="B20:E32" xr:uid="{8AF7BB84-E4B4-AE4E-877F-000F781757C1}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2631,17 +2631,17 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C40472B1-7B8C-0E47-AEDC-A96353CC7EB6}" name="li in m" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{F1F4708E-76CE-F045-B5C1-920A7D822E6B}" name="l0,schätz in m" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{6CA49B71-59FE-F749-A9F2-A92B7E8ADE00}" name="∆l0,schätz in m" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{D323358E-AC7C-6E46-88E2-1B1BA82100EA}" name="τ1 = 5 Ti in s" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{C40472B1-7B8C-0E47-AEDC-A96353CC7EB6}" name="li in m" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{F1F4708E-76CE-F045-B5C1-920A7D822E6B}" name="l0,schätz in m" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{6CA49B71-59FE-F749-A9F2-A92B7E8ADE00}" name="∆l0,schätz in m" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{D323358E-AC7C-6E46-88E2-1B1BA82100EA}" name="τ1 = 5 Ti in s" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6B02000B-784D-EB4A-9611-7F6036169ED1}" name="Table2" displayName="Table2" ref="D37:J49" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6B02000B-784D-EB4A-9611-7F6036169ED1}" name="Table2" displayName="Table2" ref="D37:J49" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="D37:J49" xr:uid="{6B02000B-784D-EB4A-9611-7F6036169ED1}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2652,34 +2652,36 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{55BB7A07-8828-5A4C-BD4B-3B1D7C9E9371}" name="∆li,Faden in m" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{CB345EF9-91E9-2047-B67F-56D715444FAC}" name="∆li,ges in m" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{F6AF1455-964D-4B4E-ADDF-86C230059387}" name="∆τ1Uhr in s" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{8F889AD9-8191-F94F-8CD2-8F439EA085FE}" name="∆τ1, ges in s" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{28B02484-B961-B74D-9AB6-9E095216CB7C}" name="Ti in s" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{55424E9E-945A-8D47-9687-E64501944523}" name="∆Ti in s" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{5EC5184E-A553-B14A-A1AB-4974E176A824}" name="∆Ti" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{55BB7A07-8828-5A4C-BD4B-3B1D7C9E9371}" name="∆li,Faden in m" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{CB345EF9-91E9-2047-B67F-56D715444FAC}" name="∆li,ges in m" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{F6AF1455-964D-4B4E-ADDF-86C230059387}" name="∆τ1Uhr in s" dataDxfId="0">
+      <calculatedColumnFormula>(0.5*E21+10)/1000</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{8F889AD9-8191-F94F-8CD2-8F439EA085FE}" name="∆τ1, ges in s" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{28B02484-B961-B74D-9AB6-9E095216CB7C}" name="Ti in s" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{55424E9E-945A-8D47-9687-E64501944523}" name="∆Ti in s" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{5EC5184E-A553-B14A-A1AB-4974E176A824}" name="∆Ti" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{73B7D59F-1C63-4547-AD26-D8CFBE8D4073}" name="Table8" displayName="Table8" ref="K37:L49" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{73B7D59F-1C63-4547-AD26-D8CFBE8D4073}" name="Table8" displayName="Table8" ref="K37:L49" totalsRowShown="0" dataDxfId="11">
   <autoFilter ref="K37:L49" xr:uid="{73B7D59F-1C63-4547-AD26-D8CFBE8D4073}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{8DB91CAB-F9B3-E542-B44E-A2119BA78EFC}" name="yi in s2" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{ACF2ADD9-FFC0-124F-A10E-AD96D23A054B}" name="∆yi in s2" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{8DB91CAB-F9B3-E542-B44E-A2119BA78EFC}" name="yi in s2" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{ACF2ADD9-FFC0-124F-A10E-AD96D23A054B}" name="∆yi in s2" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{4AAF9D21-8339-7248-AA21-DA25D233DC2D}" name="Table6" displayName="Table6" ref="B3:G5" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{4AAF9D21-8339-7248-AA21-DA25D233DC2D}" name="Table6" displayName="Table6" ref="B3:G5" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="B3:G5" xr:uid="{4AAF9D21-8339-7248-AA21-DA25D233DC2D}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2689,12 +2691,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{6261AB11-CFEF-2D47-B567-0EA7AE1B7E2B}" name=" " dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{E231D29B-F6D8-774F-9CC2-B924F00DBABA}" name="mean" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{31F917E6-C6B3-C44A-BFA1-DB5A07FB6758}" name="stdev" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{0952568A-3564-1140-91F5-02ACBC6C84C1}" name="cov" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{FCEB2C04-DB74-7347-A758-5F8318B07AC0}" name="sys" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{9BE7E060-5CB7-4E49-9CB8-F31A15C6E537}" name="total error" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{6261AB11-CFEF-2D47-B567-0EA7AE1B7E2B}" name=" " dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{E231D29B-F6D8-774F-9CC2-B924F00DBABA}" name="mean" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{31F917E6-C6B3-C44A-BFA1-DB5A07FB6758}" name="stdev" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{0952568A-3564-1140-91F5-02ACBC6C84C1}" name="cov" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{FCEB2C04-DB74-7347-A758-5F8318B07AC0}" name="sys" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{9BE7E060-5CB7-4E49-9CB8-F31A15C6E537}" name="total error" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium28" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3279,8 +3281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9FB1E29-01ED-F443-A5A0-FF909B503056}">
   <dimension ref="A1:P49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3414,7 +3416,7 @@
     </row>
     <row r="21" spans="1:7" s="1" customFormat="1" ht="22" customHeight="1">
       <c r="B21" s="14">
-        <v>2</v>
+        <v>3.25</v>
       </c>
       <c r="C21" s="8">
         <v>0.01</v>
@@ -3428,7 +3430,7 @@
     </row>
     <row r="22" spans="1:7" s="1" customFormat="1" ht="22" customHeight="1">
       <c r="B22" s="14">
-        <v>1.9</v>
+        <v>3</v>
       </c>
       <c r="C22" s="8">
         <v>0.01</v>
@@ -3445,7 +3447,7 @@
     </row>
     <row r="23" spans="1:7" s="1" customFormat="1" ht="22" customHeight="1">
       <c r="B23" s="14">
-        <v>1.8</v>
+        <v>2.75</v>
       </c>
       <c r="C23" s="8">
         <v>0.01</v>
@@ -3462,7 +3464,7 @@
     </row>
     <row r="24" spans="1:7" s="1" customFormat="1" ht="22" customHeight="1">
       <c r="B24" s="14">
-        <v>1.7</v>
+        <v>2.5</v>
       </c>
       <c r="C24" s="8">
         <v>0.01</v>
@@ -3476,7 +3478,7 @@
     </row>
     <row r="25" spans="1:7" s="1" customFormat="1" ht="22" customHeight="1">
       <c r="B25" s="14">
-        <v>1.6</v>
+        <v>2.25</v>
       </c>
       <c r="C25" s="8">
         <v>0.01</v>
@@ -3490,7 +3492,7 @@
     </row>
     <row r="26" spans="1:7" s="1" customFormat="1" ht="22" customHeight="1">
       <c r="B26" s="14">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="C26" s="8">
         <v>0.01</v>
@@ -3504,7 +3506,7 @@
     </row>
     <row r="27" spans="1:7" s="1" customFormat="1" ht="22" customHeight="1">
       <c r="B27" s="14">
-        <v>1.4</v>
+        <v>1.75</v>
       </c>
       <c r="C27" s="8">
         <v>0.01</v>
@@ -3518,7 +3520,7 @@
     </row>
     <row r="28" spans="1:7" s="1" customFormat="1" ht="22" customHeight="1">
       <c r="B28" s="14">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="C28" s="8">
         <v>0.01</v>
@@ -3532,7 +3534,7 @@
     </row>
     <row r="29" spans="1:7" s="1" customFormat="1" ht="22" customHeight="1">
       <c r="B29" s="14">
-        <v>1.2</v>
+        <v>1.25</v>
       </c>
       <c r="C29" s="8">
         <v>0.01</v>
@@ -3640,90 +3642,114 @@
     </row>
     <row r="38" spans="2:16" s="8" customFormat="1" ht="22" customHeight="1">
       <c r="B38" s="14">
-        <v>3.25</v>
+        <f>B21+C21</f>
+        <v>3.26</v>
       </c>
       <c r="C38" s="14" cm="1">
         <f t="array" ref="C38">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>0.42500000000000004</v>
+        <v>0.42600000000000005</v>
       </c>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
+      <c r="F38" s="14">
+        <f t="shared" ref="F38:F49" si="0">(0.5*E21+10)/1000</f>
+        <v>0.06</v>
+      </c>
       <c r="J38" s="19"/>
       <c r="K38" s="19"/>
       <c r="L38" s="19"/>
     </row>
     <row r="39" spans="2:16" s="8" customFormat="1" ht="22" customHeight="1">
       <c r="B39" s="14">
-        <v>3</v>
+        <f t="shared" ref="B39:B49" si="1">B22+C22</f>
+        <v>3.01</v>
       </c>
       <c r="C39" s="14" cm="1">
         <f t="array" ref="C39">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>0.4</v>
+        <v>0.40100000000000002</v>
       </c>
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
+      <c r="F39" s="14">
+        <f>(0.5*E22+10)/1000</f>
+        <v>5.5399999999999998E-2</v>
+      </c>
       <c r="J39" s="19"/>
       <c r="K39" s="19"/>
       <c r="L39" s="19"/>
     </row>
     <row r="40" spans="2:16" s="8" customFormat="1" ht="22" customHeight="1">
       <c r="B40" s="14">
-        <v>2.75</v>
+        <f t="shared" si="1"/>
+        <v>2.76</v>
       </c>
       <c r="C40" s="14" cm="1">
         <f t="array" ref="C40">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>0.375</v>
+        <v>0.376</v>
       </c>
       <c r="D40" s="14"/>
       <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
+      <c r="F40" s="14">
+        <f t="shared" si="0"/>
+        <v>5.0299999999999997E-2</v>
+      </c>
       <c r="J40" s="19"/>
       <c r="K40" s="19"/>
       <c r="L40" s="19"/>
     </row>
     <row r="41" spans="2:16" s="8" customFormat="1" ht="22" customHeight="1">
       <c r="B41" s="14">
-        <v>2.5</v>
+        <f t="shared" si="1"/>
+        <v>2.5099999999999998</v>
       </c>
       <c r="C41" s="14" cm="1">
         <f t="array" ref="C41">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>0.35</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="D41" s="14"/>
       <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
+      <c r="F41" s="14">
+        <f t="shared" si="0"/>
+        <v>4.5249999999999999E-2</v>
+      </c>
       <c r="J41" s="19"/>
       <c r="K41" s="19"/>
       <c r="L41" s="19"/>
     </row>
     <row r="42" spans="2:16" s="8" customFormat="1" ht="22" customHeight="1">
       <c r="B42" s="14">
-        <v>2.25</v>
+        <f t="shared" si="1"/>
+        <v>2.2599999999999998</v>
       </c>
       <c r="C42" s="14" cm="1">
         <f t="array" ref="C42">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>0.32500000000000001</v>
+        <v>0.32599999999999996</v>
       </c>
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
+      <c r="F42" s="14">
+        <f t="shared" si="0"/>
+        <v>4.02E-2</v>
+      </c>
       <c r="J42" s="19"/>
       <c r="K42" s="19"/>
       <c r="L42" s="19"/>
     </row>
     <row r="43" spans="2:16" s="8" customFormat="1" ht="22" customHeight="1">
       <c r="B43" s="14">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>2.0099999999999998</v>
       </c>
       <c r="C43" s="14" cm="1">
         <f t="array" ref="C43">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>0.30000000000000004</v>
+        <v>0.30099999999999999</v>
       </c>
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
+      <c r="F43" s="14">
+        <f t="shared" si="0"/>
+        <v>3.5299999999999998E-2</v>
+      </c>
       <c r="J43" s="19"/>
       <c r="K43" s="19"/>
       <c r="L43" s="19"/>
@@ -3737,15 +3763,19 @@
     </row>
     <row r="44" spans="2:16" s="8" customFormat="1" ht="22" customHeight="1">
       <c r="B44" s="14">
-        <v>1.75</v>
+        <f t="shared" si="1"/>
+        <v>1.76</v>
       </c>
       <c r="C44" s="14" cm="1">
         <f t="array" ref="C44">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>0.27500000000000002</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
+      <c r="F44" s="14">
+        <f t="shared" si="0"/>
+        <v>3.015E-2</v>
+      </c>
       <c r="J44" s="19"/>
       <c r="K44" s="19"/>
       <c r="L44" s="19"/>
@@ -3759,15 +3789,19 @@
     </row>
     <row r="45" spans="2:16" s="8" customFormat="1" ht="22" customHeight="1">
       <c r="B45" s="14">
-        <v>1.5</v>
+        <f t="shared" si="1"/>
+        <v>1.51</v>
       </c>
       <c r="C45" s="14" cm="1">
         <f t="array" ref="C45">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>0.25</v>
+        <v>0.251</v>
       </c>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
+      <c r="F45" s="14">
+        <f t="shared" si="0"/>
+        <v>2.5100000000000001E-2</v>
+      </c>
       <c r="J45" s="19"/>
       <c r="K45" s="19"/>
       <c r="L45" s="19"/>
@@ -3781,45 +3815,57 @@
     </row>
     <row r="46" spans="2:16" s="8" customFormat="1" ht="22" customHeight="1">
       <c r="B46" s="14">
-        <v>1.25</v>
+        <f t="shared" si="1"/>
+        <v>1.26</v>
       </c>
       <c r="C46" s="14" cm="1">
         <f t="array" ref="C46">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>0.22500000000000001</v>
+        <v>0.22600000000000001</v>
       </c>
       <c r="D46" s="14"/>
       <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
+      <c r="F46" s="14">
+        <f t="shared" si="0"/>
+        <v>2.0149999999999998E-2</v>
+      </c>
       <c r="J46" s="19"/>
       <c r="K46" s="19"/>
       <c r="L46" s="19"/>
     </row>
     <row r="47" spans="2:16" s="8" customFormat="1" ht="22" customHeight="1">
       <c r="B47" s="14">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>1.01</v>
       </c>
       <c r="C47" s="14" cm="1">
         <f t="array" ref="C47">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>0.2</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="D47" s="14"/>
       <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
+      <c r="F47" s="14">
+        <f t="shared" si="0"/>
+        <v>1.805E-2</v>
+      </c>
       <c r="J47" s="19"/>
       <c r="K47" s="19"/>
       <c r="L47" s="19"/>
     </row>
     <row r="48" spans="2:16" ht="22" customHeight="1">
       <c r="B48" s="14">
-        <v>0.75</v>
+        <f t="shared" si="1"/>
+        <v>1.75</v>
       </c>
       <c r="C48" s="14" cm="1">
         <f t="array" ref="C48">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>0.17500000000000002</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
+      <c r="F48" s="14">
+        <f t="shared" si="0"/>
+        <v>1.005E-2</v>
+      </c>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
       <c r="I48" s="19"/>
@@ -3829,15 +3875,19 @@
     </row>
     <row r="49" spans="2:12" ht="22" customHeight="1">
       <c r="B49" s="14">
-        <v>0.5</v>
+        <f t="shared" si="1"/>
+        <v>0.6</v>
       </c>
       <c r="C49" s="14" cm="1">
         <f t="array" ref="C49">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>0.15000000000000002</v>
+        <v>0.16</v>
       </c>
       <c r="D49" s="14"/>
       <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
+      <c r="F49" s="14">
+        <f t="shared" si="0"/>
+        <v>1.005E-2</v>
+      </c>
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
       <c r="I49" s="19"/>

</xml_diff>

<commit_message>
pls make the plot prettier
</commit_message>
<xml_diff>
--- a/Pendulum/F3_Fadenpendel.xlsx
+++ b/Pendulum/F3_Fadenpendel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huyenanh/git_repos/MB14_Classical_mechanics/Pendulum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D419F713-C4D3-3C4E-928D-F67FC65B3BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEBA7EC-3813-FF49-8D05-EF1DD1B273C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="760" windowWidth="28300" windowHeight="18880" activeTab="1" xr2:uid="{0C87622E-8A3E-9447-883B-E874DD3727AC}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="84">
   <si>
     <t>l = Fadenlänge</t>
   </si>
@@ -786,6 +786,30 @@
       </rPr>
       <t>2</t>
     </r>
+  </si>
+  <si>
+    <t>Fadenlänge</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>+ 21.5 cm</t>
+  </si>
+  <si>
+    <t>Grad</t>
+  </si>
+  <si>
+    <t>Anh</t>
+  </si>
+  <si>
+    <t>Maksims</t>
+  </si>
+  <si>
+    <t>Oscar</t>
+  </si>
+  <si>
+    <t>0.01 s abweichung</t>
   </si>
 </sst>
 </file>
@@ -898,7 +922,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -917,8 +941,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor theme="6" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor theme="6" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -926,11 +962,59 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -981,15 +1065,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="38">
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1054,6 +1155,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2654,34 +2759,34 @@
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{55BB7A07-8828-5A4C-BD4B-3B1D7C9E9371}" name="∆li,Faden in m" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{CB345EF9-91E9-2047-B67F-56D715444FAC}" name="∆li,ges in m" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{F6AF1455-964D-4B4E-ADDF-86C230059387}" name="∆τ1Uhr in s" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{F6AF1455-964D-4B4E-ADDF-86C230059387}" name="∆τ1Uhr in s" dataDxfId="15">
       <calculatedColumnFormula>(0.5*E21+10)/1000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8F889AD9-8191-F94F-8CD2-8F439EA085FE}" name="∆τ1, ges in s" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{28B02484-B961-B74D-9AB6-9E095216CB7C}" name="Ti in s" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{55424E9E-945A-8D47-9687-E64501944523}" name="∆Ti in s" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{5EC5184E-A553-B14A-A1AB-4974E176A824}" name="∆Ti" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{8F889AD9-8191-F94F-8CD2-8F439EA085FE}" name="∆τ1, ges in s" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{28B02484-B961-B74D-9AB6-9E095216CB7C}" name="Ti in s" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{55424E9E-945A-8D47-9687-E64501944523}" name="∆Ti in s" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{5EC5184E-A553-B14A-A1AB-4974E176A824}" name="∆Ti" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{73B7D59F-1C63-4547-AD26-D8CFBE8D4073}" name="Table8" displayName="Table8" ref="K37:L49" totalsRowShown="0" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{73B7D59F-1C63-4547-AD26-D8CFBE8D4073}" name="Table8" displayName="Table8" ref="K37:L49" totalsRowShown="0" dataDxfId="10">
   <autoFilter ref="K37:L49" xr:uid="{73B7D59F-1C63-4547-AD26-D8CFBE8D4073}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{8DB91CAB-F9B3-E542-B44E-A2119BA78EFC}" name="yi in s2" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{ACF2ADD9-FFC0-124F-A10E-AD96D23A054B}" name="∆yi in s2" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{8DB91CAB-F9B3-E542-B44E-A2119BA78EFC}" name="yi in s2" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{ACF2ADD9-FFC0-124F-A10E-AD96D23A054B}" name="∆yi in s2" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{4AAF9D21-8339-7248-AA21-DA25D233DC2D}" name="Table6" displayName="Table6" ref="B3:G5" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{4AAF9D21-8339-7248-AA21-DA25D233DC2D}" name="Table6" displayName="Table6" ref="B3:G5" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="B3:G5" xr:uid="{4AAF9D21-8339-7248-AA21-DA25D233DC2D}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2691,12 +2796,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{6261AB11-CFEF-2D47-B567-0EA7AE1B7E2B}" name=" " dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{E231D29B-F6D8-774F-9CC2-B924F00DBABA}" name="mean" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{31F917E6-C6B3-C44A-BFA1-DB5A07FB6758}" name="stdev" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{0952568A-3564-1140-91F5-02ACBC6C84C1}" name="cov" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{FCEB2C04-DB74-7347-A758-5F8318B07AC0}" name="sys" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{9BE7E060-5CB7-4E49-9CB8-F31A15C6E537}" name="total error" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{6261AB11-CFEF-2D47-B567-0EA7AE1B7E2B}" name=" " dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{E231D29B-F6D8-774F-9CC2-B924F00DBABA}" name="mean" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{31F917E6-C6B3-C44A-BFA1-DB5A07FB6758}" name="stdev" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{0952568A-3564-1140-91F5-02ACBC6C84C1}" name="cov" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{FCEB2C04-DB74-7347-A758-5F8318B07AC0}" name="sys" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{9BE7E060-5CB7-4E49-9CB8-F31A15C6E537}" name="total error" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium28" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3279,10 +3384,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9FB1E29-01ED-F443-A5A0-FF909B503056}">
-  <dimension ref="A1:P49"/>
+  <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3297,110 +3402,274 @@
     <col min="8" max="8" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="12" customFormat="1" ht="16">
+    <row r="1" spans="1:19" s="12" customFormat="1" ht="16">
       <c r="A1" s="12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="8" customFormat="1" ht="24" customHeight="1">
+    <row r="3" spans="1:19" s="8" customFormat="1" ht="24" customHeight="1">
       <c r="B3" s="11" t="s">
         <v>44</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" s="8" customFormat="1" ht="17" customHeight="1">
+      <c r="L3" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" s="8" customFormat="1" ht="17" customHeight="1">
       <c r="B4" s="14">
-        <v>1.2</v>
+        <v>2.96</v>
       </c>
       <c r="C4" s="14">
+        <v>2.75</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="8">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" s="8" customFormat="1" ht="17" customHeight="1">
+      <c r="G4" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="L4" s="23">
+        <v>3.34</v>
+      </c>
+      <c r="M4" s="24">
+        <v>2.71</v>
+      </c>
+      <c r="O4" s="23">
+        <v>2.96</v>
+      </c>
+      <c r="P4" s="24">
+        <v>2.75</v>
+      </c>
+      <c r="R4" s="23"/>
+      <c r="S4" s="24"/>
+    </row>
+    <row r="5" spans="1:19" s="8" customFormat="1" ht="17" customHeight="1">
       <c r="B5" s="14">
-        <v>1.1000000000000001</v>
+        <v>3.13</v>
       </c>
       <c r="C5" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="8" customFormat="1" ht="17" customHeight="1">
+        <v>2.96</v>
+      </c>
+      <c r="L5" s="25">
+        <v>3.13</v>
+      </c>
+      <c r="M5" s="26">
+        <v>2.75</v>
+      </c>
+      <c r="O5" s="25">
+        <v>3.13</v>
+      </c>
+      <c r="P5" s="26">
+        <v>2.96</v>
+      </c>
+      <c r="R5" s="25"/>
+      <c r="S5" s="26"/>
+    </row>
+    <row r="6" spans="1:19" s="8" customFormat="1" ht="17" customHeight="1">
       <c r="B6" s="14">
-        <v>1</v>
+        <v>3.13</v>
       </c>
       <c r="C6" s="14">
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="8" customFormat="1" ht="17" customHeight="1">
+        <v>2.95</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="L6" s="23">
+        <v>3.17</v>
+      </c>
+      <c r="M6" s="24">
+        <v>2.88</v>
+      </c>
+      <c r="O6" s="23">
+        <v>3.13</v>
+      </c>
+      <c r="P6" s="24">
+        <v>2.95</v>
+      </c>
+      <c r="R6" s="23"/>
+      <c r="S6" s="24"/>
+    </row>
+    <row r="7" spans="1:19" s="8" customFormat="1" ht="17" customHeight="1">
       <c r="B7" s="14">
-        <v>0.9</v>
+        <v>3.25</v>
       </c>
       <c r="C7" s="14">
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="8" customFormat="1" ht="17" customHeight="1">
+        <v>2.96</v>
+      </c>
+      <c r="L7" s="25">
+        <v>3.15</v>
+      </c>
+      <c r="M7" s="26">
+        <v>2.93</v>
+      </c>
+      <c r="O7" s="25">
+        <v>3.25</v>
+      </c>
+      <c r="P7" s="26">
+        <v>2.96</v>
+      </c>
+      <c r="R7" s="25"/>
+      <c r="S7" s="26"/>
+    </row>
+    <row r="8" spans="1:19" s="8" customFormat="1" ht="17" customHeight="1">
       <c r="B8" s="14">
-        <v>1.2</v>
+        <v>3.08</v>
       </c>
       <c r="C8" s="14">
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" s="8" customFormat="1" ht="17" customHeight="1">
+        <v>3.1</v>
+      </c>
+      <c r="L8" s="23">
+        <v>3.22</v>
+      </c>
+      <c r="M8" s="24">
+        <v>2.95</v>
+      </c>
+      <c r="O8" s="23">
+        <v>3.08</v>
+      </c>
+      <c r="P8" s="24">
+        <v>3.1</v>
+      </c>
+      <c r="R8" s="23"/>
+      <c r="S8" s="24"/>
+    </row>
+    <row r="9" spans="1:19" s="8" customFormat="1" ht="17" customHeight="1">
       <c r="B9" s="14">
-        <v>1.2</v>
+        <v>3.08</v>
       </c>
       <c r="C9" s="14">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="8" customFormat="1" ht="17" customHeight="1">
+        <v>3.18</v>
+      </c>
+      <c r="L9" s="25">
+        <v>3.13</v>
+      </c>
+      <c r="M9" s="26">
+        <v>2.88</v>
+      </c>
+      <c r="O9" s="25">
+        <v>3.08</v>
+      </c>
+      <c r="P9" s="26">
+        <v>3.18</v>
+      </c>
+      <c r="R9" s="25"/>
+      <c r="S9" s="26"/>
+    </row>
+    <row r="10" spans="1:19" s="8" customFormat="1" ht="17" customHeight="1">
       <c r="B10" s="14">
-        <v>1.1000000000000001</v>
+        <v>3.03</v>
       </c>
       <c r="C10" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="8" customFormat="1" ht="17" customHeight="1">
+        <v>3.08</v>
+      </c>
+      <c r="L10" s="23">
+        <v>3.12</v>
+      </c>
+      <c r="M10" s="24">
+        <v>2.95</v>
+      </c>
+      <c r="O10" s="23">
+        <v>3.03</v>
+      </c>
+      <c r="P10" s="24">
+        <v>3.08</v>
+      </c>
+      <c r="R10" s="23"/>
+      <c r="S10" s="24"/>
+    </row>
+    <row r="11" spans="1:19" s="8" customFormat="1" ht="17" customHeight="1">
       <c r="B11" s="14">
-        <v>0.9</v>
+        <v>3.11</v>
       </c>
       <c r="C11" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="8" customFormat="1" ht="17" customHeight="1">
+        <v>3.11</v>
+      </c>
+      <c r="L11" s="25">
+        <v>3.1</v>
+      </c>
+      <c r="M11" s="26">
+        <v>2.81</v>
+      </c>
+      <c r="O11" s="25">
+        <v>3.11</v>
+      </c>
+      <c r="P11" s="26">
+        <v>3.11</v>
+      </c>
+      <c r="R11" s="25"/>
+      <c r="S11" s="26"/>
+    </row>
+    <row r="12" spans="1:19" s="8" customFormat="1" ht="17" customHeight="1">
       <c r="B12" s="14">
-        <v>1</v>
+        <v>3.13</v>
       </c>
       <c r="C12" s="14">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="8" customFormat="1" ht="17" customHeight="1">
+        <v>3.08</v>
+      </c>
+      <c r="L12" s="23">
+        <v>3.07</v>
+      </c>
+      <c r="M12" s="24">
+        <v>2.89</v>
+      </c>
+      <c r="O12" s="23">
+        <v>3.13</v>
+      </c>
+      <c r="P12" s="24">
+        <v>3.08</v>
+      </c>
+      <c r="R12" s="23"/>
+      <c r="S12" s="24"/>
+    </row>
+    <row r="13" spans="1:19" s="8" customFormat="1" ht="17" customHeight="1">
       <c r="B13" s="14">
-        <v>1</v>
+        <v>3.13</v>
       </c>
       <c r="C13" s="14">
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="17">
+        <v>2.98</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="L13" s="27">
+        <v>3.01</v>
+      </c>
+      <c r="M13" s="28">
+        <v>2.97</v>
+      </c>
+      <c r="O13" s="27">
+        <v>3.13</v>
+      </c>
+      <c r="P13" s="28">
+        <v>2.98</v>
+      </c>
+      <c r="R13" s="27"/>
+      <c r="S13" s="28"/>
+    </row>
+    <row r="15" spans="1:19" ht="17">
       <c r="B15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="13" customFormat="1" ht="16">
+    <row r="18" spans="1:9" s="13" customFormat="1" ht="16">
       <c r="A18" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" ht="26" customHeight="1">
+    <row r="20" spans="1:9" s="1" customFormat="1" ht="26" customHeight="1">
       <c r="B20" s="8" t="s">
         <v>54</v>
       </c>
@@ -3414,178 +3683,184 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="1" customFormat="1" ht="22" customHeight="1">
+    <row r="21" spans="1:9" s="1" customFormat="1" ht="22" customHeight="1">
       <c r="B21" s="14">
-        <v>3.25</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="C21" s="8">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D21" s="8">
         <v>0.01</v>
       </c>
-      <c r="D21" s="8">
-        <v>1E-3</v>
-      </c>
       <c r="E21" s="8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" ht="22" customHeight="1">
+        <v>14.83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="1" customFormat="1" ht="22" customHeight="1">
       <c r="B22" s="14">
-        <v>3</v>
+        <v>1.93</v>
       </c>
       <c r="C22" s="8">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D22" s="8">
         <v>0.01</v>
       </c>
-      <c r="D22" s="8">
-        <v>1E-3</v>
-      </c>
       <c r="E22" s="8">
-        <v>90.8</v>
+        <v>14.44</v>
       </c>
       <c r="G22" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" s="1" customFormat="1" ht="22" customHeight="1">
+      <c r="H22" s="1">
+        <v>10</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="1" customFormat="1" ht="22" customHeight="1">
       <c r="B23" s="14">
-        <v>2.75</v>
+        <v>1.83</v>
       </c>
       <c r="C23" s="8">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D23" s="8">
         <v>0.01</v>
       </c>
-      <c r="D23" s="8">
-        <v>1E-3</v>
-      </c>
       <c r="E23" s="8">
-        <v>80.599999999999994</v>
+        <v>14.11</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="1" customFormat="1" ht="22" customHeight="1">
+    <row r="24" spans="1:9" s="1" customFormat="1" ht="22" customHeight="1">
       <c r="B24" s="14">
-        <v>2.5</v>
+        <v>1.73</v>
       </c>
       <c r="C24" s="8">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D24" s="8">
         <v>0.01</v>
       </c>
-      <c r="D24" s="8">
-        <v>1E-3</v>
-      </c>
       <c r="E24" s="8">
-        <v>70.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" s="1" customFormat="1" ht="22" customHeight="1">
+        <v>13.71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="1" customFormat="1" ht="22" customHeight="1">
       <c r="B25" s="14">
-        <v>2.25</v>
+        <v>1.63</v>
       </c>
       <c r="C25" s="8">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D25" s="8">
         <v>0.01</v>
       </c>
-      <c r="D25" s="8">
-        <v>1E-3</v>
-      </c>
       <c r="E25" s="8">
-        <v>60.4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" s="1" customFormat="1" ht="22" customHeight="1">
+        <v>13.29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="1" customFormat="1" ht="22" customHeight="1">
       <c r="B26" s="14">
-        <v>2</v>
+        <v>1.53</v>
       </c>
       <c r="C26" s="8">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D26" s="8">
         <v>0.01</v>
       </c>
-      <c r="D26" s="8">
-        <v>1E-3</v>
-      </c>
       <c r="E26" s="8">
-        <v>50.6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" s="1" customFormat="1" ht="22" customHeight="1">
+        <v>13.09</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="1" customFormat="1" ht="22" customHeight="1">
       <c r="B27" s="14">
-        <v>1.75</v>
+        <v>1.43</v>
       </c>
       <c r="C27" s="8">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D27" s="8">
         <v>0.01</v>
       </c>
-      <c r="D27" s="8">
-        <v>1E-3</v>
-      </c>
       <c r="E27" s="8">
-        <v>40.299999999999997</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="1" customFormat="1" ht="22" customHeight="1">
+        <v>12.58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="1" customFormat="1" ht="22" customHeight="1">
       <c r="B28" s="14">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
       <c r="C28" s="8">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D28" s="8">
         <v>0.01</v>
       </c>
-      <c r="D28" s="8">
-        <v>1E-3</v>
-      </c>
       <c r="E28" s="8">
-        <v>30.2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" s="1" customFormat="1" ht="22" customHeight="1">
+        <v>12.17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="1" customFormat="1" ht="22" customHeight="1">
       <c r="B29" s="14">
-        <v>1.25</v>
+        <v>1.23</v>
       </c>
       <c r="C29" s="8">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D29" s="8">
         <v>0.01</v>
       </c>
-      <c r="D29" s="8">
-        <v>1E-3</v>
-      </c>
       <c r="E29" s="8">
-        <v>20.3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" s="1" customFormat="1" ht="22" customHeight="1">
+        <v>11.77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="1" customFormat="1" ht="22" customHeight="1">
       <c r="B30" s="14">
-        <v>1</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="C30" s="8">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D30" s="8">
         <v>0.01</v>
       </c>
-      <c r="D30" s="8">
-        <v>1E-3</v>
-      </c>
       <c r="E30" s="8">
-        <v>16.100000000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="22" customHeight="1">
+        <v>11.27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="22" customHeight="1">
       <c r="B31" s="14">
-        <v>0.75</v>
+        <v>1.03</v>
       </c>
       <c r="C31" s="8">
-        <v>1</v>
+        <v>1.2E-2</v>
       </c>
       <c r="D31" s="8">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E31" s="8">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="22" customHeight="1">
+        <v>10.95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="22" customHeight="1">
       <c r="B32" s="14">
-        <v>0.5</v>
+        <v>0.93</v>
       </c>
       <c r="C32" s="8">
-        <v>0.1</v>
+        <v>1.2E-2</v>
       </c>
       <c r="D32" s="8">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E32" s="8">
-        <v>0.1</v>
+        <v>10.55</v>
       </c>
     </row>
     <row r="33" spans="2:16">
@@ -3643,17 +3918,17 @@
     <row r="38" spans="2:16" s="8" customFormat="1" ht="22" customHeight="1">
       <c r="B38" s="14">
         <f>B21+C21</f>
-        <v>3.26</v>
+        <v>2.0419999999999998</v>
       </c>
       <c r="C38" s="14" cm="1">
         <f t="array" ref="C38">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>0.42600000000000005</v>
+        <v>1.4167999999999998</v>
       </c>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
       <c r="F38" s="14">
         <f t="shared" ref="F38:F49" si="0">(0.5*E21+10)/1000</f>
-        <v>0.06</v>
+        <v>1.7415E-2</v>
       </c>
       <c r="J38" s="19"/>
       <c r="K38" s="19"/>
@@ -3661,18 +3936,18 @@
     </row>
     <row r="39" spans="2:16" s="8" customFormat="1" ht="22" customHeight="1">
       <c r="B39" s="14">
-        <f t="shared" ref="B39:B49" si="1">B22+C22</f>
-        <v>3.01</v>
+        <f>B22+C22</f>
+        <v>1.9419999999999999</v>
       </c>
       <c r="C39" s="14" cm="1">
         <f t="array" ref="C39">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>0.40100000000000002</v>
+        <v>1.3768</v>
       </c>
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
       <c r="F39" s="14">
         <f>(0.5*E22+10)/1000</f>
-        <v>5.5399999999999998E-2</v>
+        <v>1.7219999999999999E-2</v>
       </c>
       <c r="J39" s="19"/>
       <c r="K39" s="19"/>
@@ -3680,18 +3955,18 @@
     </row>
     <row r="40" spans="2:16" s="8" customFormat="1" ht="22" customHeight="1">
       <c r="B40" s="14">
-        <f t="shared" si="1"/>
-        <v>2.76</v>
+        <f t="shared" ref="B40:B49" si="1">B23+C23</f>
+        <v>1.8420000000000001</v>
       </c>
       <c r="C40" s="14" cm="1">
         <f t="array" ref="C40">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>0.376</v>
+        <v>1.3368000000000002</v>
       </c>
       <c r="D40" s="14"/>
       <c r="E40" s="14"/>
       <c r="F40" s="14">
         <f t="shared" si="0"/>
-        <v>5.0299999999999997E-2</v>
+        <v>1.7055000000000001E-2</v>
       </c>
       <c r="J40" s="19"/>
       <c r="K40" s="19"/>
@@ -3700,17 +3975,17 @@
     <row r="41" spans="2:16" s="8" customFormat="1" ht="22" customHeight="1">
       <c r="B41" s="14">
         <f t="shared" si="1"/>
-        <v>2.5099999999999998</v>
+        <v>1.742</v>
       </c>
       <c r="C41" s="14" cm="1">
         <f t="array" ref="C41">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>0.35099999999999998</v>
+        <v>1.2968000000000002</v>
       </c>
       <c r="D41" s="14"/>
       <c r="E41" s="14"/>
       <c r="F41" s="14">
         <f t="shared" si="0"/>
-        <v>4.5249999999999999E-2</v>
+        <v>1.6855000000000002E-2</v>
       </c>
       <c r="J41" s="19"/>
       <c r="K41" s="19"/>
@@ -3719,17 +3994,17 @@
     <row r="42" spans="2:16" s="8" customFormat="1" ht="22" customHeight="1">
       <c r="B42" s="14">
         <f t="shared" si="1"/>
-        <v>2.2599999999999998</v>
+        <v>1.6419999999999999</v>
       </c>
       <c r="C42" s="14" cm="1">
         <f t="array" ref="C42">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>0.32599999999999996</v>
+        <v>1.2568000000000001</v>
       </c>
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
       <c r="F42" s="14">
         <f t="shared" si="0"/>
-        <v>4.02E-2</v>
+        <v>1.6645E-2</v>
       </c>
       <c r="J42" s="19"/>
       <c r="K42" s="19"/>
@@ -3738,17 +4013,17 @@
     <row r="43" spans="2:16" s="8" customFormat="1" ht="22" customHeight="1">
       <c r="B43" s="14">
         <f t="shared" si="1"/>
-        <v>2.0099999999999998</v>
+        <v>1.542</v>
       </c>
       <c r="C43" s="14" cm="1">
         <f t="array" ref="C43">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>0.30099999999999999</v>
+        <v>1.2168000000000001</v>
       </c>
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
       <c r="F43" s="14">
         <f t="shared" si="0"/>
-        <v>3.5299999999999998E-2</v>
+        <v>1.6545000000000001E-2</v>
       </c>
       <c r="J43" s="19"/>
       <c r="K43" s="19"/>
@@ -3758,23 +4033,23 @@
       </c>
       <c r="O43" s="3"/>
       <c r="P43" s="18">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="2:16" s="8" customFormat="1" ht="22" customHeight="1">
       <c r="B44" s="14">
         <f t="shared" si="1"/>
-        <v>1.76</v>
+        <v>1.4419999999999999</v>
       </c>
       <c r="C44" s="14" cm="1">
         <f t="array" ref="C44">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>0.27600000000000002</v>
+        <v>1.1768000000000001</v>
       </c>
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
       <c r="F44" s="14">
         <f t="shared" si="0"/>
-        <v>3.015E-2</v>
+        <v>1.6289999999999999E-2</v>
       </c>
       <c r="J44" s="19"/>
       <c r="K44" s="19"/>
@@ -3790,43 +4065,43 @@
     <row r="45" spans="2:16" s="8" customFormat="1" ht="22" customHeight="1">
       <c r="B45" s="14">
         <f t="shared" si="1"/>
-        <v>1.51</v>
+        <v>1.3420000000000001</v>
       </c>
       <c r="C45" s="14" cm="1">
         <f t="array" ref="C45">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>0.251</v>
+        <v>1.1368</v>
       </c>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
       <c r="F45" s="14">
         <f t="shared" si="0"/>
-        <v>2.5100000000000001E-2</v>
+        <v>1.6085000000000002E-2</v>
       </c>
       <c r="J45" s="19"/>
       <c r="K45" s="19"/>
       <c r="L45" s="19"/>
       <c r="N45" s="15"/>
       <c r="O45" s="15">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
       <c r="P45" s="15">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="46" spans="2:16" s="8" customFormat="1" ht="22" customHeight="1">
       <c r="B46" s="14">
         <f t="shared" si="1"/>
-        <v>1.26</v>
+        <v>1.242</v>
       </c>
       <c r="C46" s="14" cm="1">
         <f t="array" ref="C46">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>0.22600000000000001</v>
+        <v>1.0968</v>
       </c>
       <c r="D46" s="14"/>
       <c r="E46" s="14"/>
       <c r="F46" s="14">
         <f t="shared" si="0"/>
-        <v>2.0149999999999998E-2</v>
+        <v>1.5885E-2</v>
       </c>
       <c r="J46" s="19"/>
       <c r="K46" s="19"/>
@@ -3835,17 +4110,17 @@
     <row r="47" spans="2:16" s="8" customFormat="1" ht="22" customHeight="1">
       <c r="B47" s="14">
         <f t="shared" si="1"/>
-        <v>1.01</v>
+        <v>1.1419999999999999</v>
       </c>
       <c r="C47" s="14" cm="1">
         <f t="array" ref="C47">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>0.20100000000000001</v>
+        <v>1.0568</v>
       </c>
       <c r="D47" s="14"/>
       <c r="E47" s="14"/>
       <c r="F47" s="14">
         <f t="shared" si="0"/>
-        <v>1.805E-2</v>
+        <v>1.5635E-2</v>
       </c>
       <c r="J47" s="19"/>
       <c r="K47" s="19"/>
@@ -3854,17 +4129,17 @@
     <row r="48" spans="2:16" ht="22" customHeight="1">
       <c r="B48" s="14">
         <f t="shared" si="1"/>
-        <v>1.75</v>
+        <v>1.042</v>
       </c>
       <c r="C48" s="14" cm="1">
         <f t="array" ref="C48">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>0.27500000000000002</v>
+        <v>1.0167999999999999</v>
       </c>
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
       <c r="F48" s="14">
         <f t="shared" si="0"/>
-        <v>1.005E-2</v>
+        <v>1.5474999999999999E-2</v>
       </c>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
@@ -3876,17 +4151,17 @@
     <row r="49" spans="2:12" ht="22" customHeight="1">
       <c r="B49" s="14">
         <f t="shared" si="1"/>
-        <v>0.6</v>
+        <v>0.94200000000000006</v>
       </c>
       <c r="C49" s="14" cm="1">
         <f t="array" ref="C49">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>0.16</v>
+        <v>0.9768</v>
       </c>
       <c r="D49" s="14"/>
       <c r="E49" s="14"/>
       <c r="F49" s="14">
         <f t="shared" si="0"/>
-        <v>1.005E-2</v>
+        <v>1.5275E-2</v>
       </c>
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>

</xml_diff>

<commit_message>
label and horizontal errorbar
</commit_message>
<xml_diff>
--- a/Pendulum/F3_Fadenpendel.xlsx
+++ b/Pendulum/F3_Fadenpendel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huyenanh/git_repos/MB14_Classical_mechanics/Pendulum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEBA7EC-3813-FF49-8D05-EF1DD1B273C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBF8D8E-6B6A-F941-89F2-5912F472558B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="760" windowWidth="28300" windowHeight="18880" activeTab="1" xr2:uid="{0C87622E-8A3E-9447-883B-E874DD3727AC}"/>
+    <workbookView xWindow="1200" yWindow="760" windowWidth="28300" windowHeight="18880" activeTab="2" xr2:uid="{0C87622E-8A3E-9447-883B-E874DD3727AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Durchführung" sheetId="3" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="83">
   <si>
     <t>l = Fadenlänge</t>
   </si>
@@ -450,9 +450,6 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Versuchsteil 3: 10 Perioden  bei 10 unterschiedlichen Pendellänge</t>
   </si>
   <si>
     <r>
@@ -3386,8 +3383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9FB1E29-01ED-F443-A5A0-FF909B503056}">
   <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3415,13 +3412,13 @@
         <v>45</v>
       </c>
       <c r="L3" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="O3" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="R3" s="8" t="s">
         <v>81</v>
-      </c>
-      <c r="R3" s="8" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:19" s="8" customFormat="1" ht="17" customHeight="1">
@@ -3432,13 +3429,13 @@
         <v>2.75</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F4" s="8">
         <v>2.1</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L4" s="23">
         <v>3.34</v>
@@ -3485,7 +3482,7 @@
         <v>2.95</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L6" s="23">
         <v>3.17</v>
@@ -3642,7 +3639,7 @@
         <v>2.98</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L13" s="27">
         <v>3.01</v>
@@ -3666,7 +3663,7 @@
     </row>
     <row r="18" spans="1:9" s="13" customFormat="1" ht="16">
       <c r="A18" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="1" customFormat="1" ht="26" customHeight="1">
@@ -3680,7 +3677,7 @@
         <v>55</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="1" customFormat="1" ht="22" customHeight="1">
@@ -3691,7 +3688,7 @@
         <v>1.2E-2</v>
       </c>
       <c r="D21" s="8">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="E21" s="8">
         <v>14.83</v>
@@ -3705,7 +3702,7 @@
         <v>1.2E-2</v>
       </c>
       <c r="D22" s="8">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="E22" s="8">
         <v>14.44</v>
@@ -3717,7 +3714,7 @@
         <v>10</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="1" customFormat="1" ht="22" customHeight="1">
@@ -3728,7 +3725,7 @@
         <v>1.2E-2</v>
       </c>
       <c r="D23" s="8">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="E23" s="8">
         <v>14.11</v>
@@ -3745,7 +3742,7 @@
         <v>1.2E-2</v>
       </c>
       <c r="D24" s="8">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="E24" s="8">
         <v>13.71</v>
@@ -3759,7 +3756,7 @@
         <v>1.2E-2</v>
       </c>
       <c r="D25" s="8">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="E25" s="8">
         <v>13.29</v>
@@ -3773,7 +3770,7 @@
         <v>1.2E-2</v>
       </c>
       <c r="D26" s="8">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="E26" s="8">
         <v>13.09</v>
@@ -3787,7 +3784,7 @@
         <v>1.2E-2</v>
       </c>
       <c r="D27" s="8">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="E27" s="8">
         <v>12.58</v>
@@ -3801,7 +3798,7 @@
         <v>1.2E-2</v>
       </c>
       <c r="D28" s="8">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="E28" s="8">
         <v>12.17</v>
@@ -3815,7 +3812,7 @@
         <v>1.2E-2</v>
       </c>
       <c r="D29" s="8">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="E29" s="8">
         <v>11.77</v>
@@ -3829,7 +3826,7 @@
         <v>1.2E-2</v>
       </c>
       <c r="D30" s="8">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="E30" s="8">
         <v>11.27</v>
@@ -3843,7 +3840,7 @@
         <v>1.2E-2</v>
       </c>
       <c r="D31" s="8">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="E31" s="8">
         <v>10.95</v>
@@ -3857,7 +3854,7 @@
         <v>1.2E-2</v>
       </c>
       <c r="D32" s="8">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="E32" s="8">
         <v>10.55</v>
@@ -3882,37 +3879,37 @@
     </row>
     <row r="37" spans="2:16" s="8" customFormat="1" ht="24" customHeight="1">
       <c r="B37" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D37" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="E37" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="E37" s="21" t="s">
+      <c r="F37" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="F37" s="21" t="s">
+      <c r="G37" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="G37" s="21" t="s">
+      <c r="H37" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="H37" s="21" t="s">
+      <c r="I37" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="I37" s="21" t="s">
+      <c r="J37" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="J37" s="21" t="s">
+      <c r="K37" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="L37" s="11" t="s">
         <v>74</v>
-      </c>
-      <c r="K37" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="L37" s="11" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="38" spans="2:16" s="8" customFormat="1" ht="22" customHeight="1">
@@ -3920,9 +3917,9 @@
         <f>B21+C21</f>
         <v>2.0419999999999998</v>
       </c>
-      <c r="C38" s="14" cm="1">
-        <f t="array" ref="C38">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>1.4167999999999998</v>
+      <c r="C38" s="19" cm="1">
+        <f t="array" ref="C38">(Table5[b]/1000*Table4[[#This Row],[li,ges in m]]) + Table5[a]/1000</f>
+        <v>1.4168E-3</v>
       </c>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
@@ -3939,9 +3936,9 @@
         <f>B22+C22</f>
         <v>1.9419999999999999</v>
       </c>
-      <c r="C39" s="14" cm="1">
-        <f t="array" ref="C39">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>1.3768</v>
+      <c r="C39" s="19" cm="1">
+        <f t="array" ref="C39">(Table5[b]/1000*Table4[[#This Row],[li,ges in m]]) + Table5[a]/1000</f>
+        <v>1.3768000000000001E-3</v>
       </c>
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
@@ -3958,9 +3955,9 @@
         <f t="shared" ref="B40:B49" si="1">B23+C23</f>
         <v>1.8420000000000001</v>
       </c>
-      <c r="C40" s="14" cm="1">
-        <f t="array" ref="C40">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>1.3368000000000002</v>
+      <c r="C40" s="19" cm="1">
+        <f t="array" ref="C40">(Table5[b]/1000*Table4[[#This Row],[li,ges in m]]) + Table5[a]/1000</f>
+        <v>1.3368E-3</v>
       </c>
       <c r="D40" s="14"/>
       <c r="E40" s="14"/>
@@ -3977,9 +3974,9 @@
         <f t="shared" si="1"/>
         <v>1.742</v>
       </c>
-      <c r="C41" s="14" cm="1">
-        <f t="array" ref="C41">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>1.2968000000000002</v>
+      <c r="C41" s="19" cm="1">
+        <f t="array" ref="C41">(Table5[b]/1000*Table4[[#This Row],[li,ges in m]]) + Table5[a]/1000</f>
+        <v>1.2967999999999999E-3</v>
       </c>
       <c r="D41" s="14"/>
       <c r="E41" s="14"/>
@@ -3996,9 +3993,9 @@
         <f t="shared" si="1"/>
         <v>1.6419999999999999</v>
       </c>
-      <c r="C42" s="14" cm="1">
-        <f t="array" ref="C42">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>1.2568000000000001</v>
+      <c r="C42" s="19" cm="1">
+        <f t="array" ref="C42">(Table5[b]/1000*Table4[[#This Row],[li,ges in m]]) + Table5[a]/1000</f>
+        <v>1.2568E-3</v>
       </c>
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
@@ -4015,9 +4012,9 @@
         <f t="shared" si="1"/>
         <v>1.542</v>
       </c>
-      <c r="C43" s="14" cm="1">
-        <f t="array" ref="C43">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>1.2168000000000001</v>
+      <c r="C43" s="19" cm="1">
+        <f t="array" ref="C43">(Table5[b]/1000*Table4[[#This Row],[li,ges in m]]) + Table5[a]/1000</f>
+        <v>1.2168000000000001E-3</v>
       </c>
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
@@ -4041,9 +4038,9 @@
         <f t="shared" si="1"/>
         <v>1.4419999999999999</v>
       </c>
-      <c r="C44" s="14" cm="1">
-        <f t="array" ref="C44">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>1.1768000000000001</v>
+      <c r="C44" s="19" cm="1">
+        <f t="array" ref="C44">(Table5[b]/1000*Table4[[#This Row],[li,ges in m]]) + Table5[a]/1000</f>
+        <v>1.1768E-3</v>
       </c>
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
@@ -4067,9 +4064,9 @@
         <f t="shared" si="1"/>
         <v>1.3420000000000001</v>
       </c>
-      <c r="C45" s="14" cm="1">
-        <f t="array" ref="C45">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>1.1368</v>
+      <c r="C45" s="19" cm="1">
+        <f t="array" ref="C45">(Table5[b]/1000*Table4[[#This Row],[li,ges in m]]) + Table5[a]/1000</f>
+        <v>1.1367999999999999E-3</v>
       </c>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
@@ -4093,9 +4090,9 @@
         <f t="shared" si="1"/>
         <v>1.242</v>
       </c>
-      <c r="C46" s="14" cm="1">
-        <f t="array" ref="C46">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>1.0968</v>
+      <c r="C46" s="19" cm="1">
+        <f t="array" ref="C46">(Table5[b]/1000*Table4[[#This Row],[li,ges in m]]) + Table5[a]/1000</f>
+        <v>1.0968E-3</v>
       </c>
       <c r="D46" s="14"/>
       <c r="E46" s="14"/>
@@ -4112,9 +4109,9 @@
         <f t="shared" si="1"/>
         <v>1.1419999999999999</v>
       </c>
-      <c r="C47" s="14" cm="1">
-        <f t="array" ref="C47">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>1.0568</v>
+      <c r="C47" s="19" cm="1">
+        <f t="array" ref="C47">(Table5[b]/1000*Table4[[#This Row],[li,ges in m]]) + Table5[a]/1000</f>
+        <v>1.0567999999999999E-3</v>
       </c>
       <c r="D47" s="14"/>
       <c r="E47" s="14"/>
@@ -4131,9 +4128,9 @@
         <f t="shared" si="1"/>
         <v>1.042</v>
       </c>
-      <c r="C48" s="14" cm="1">
-        <f t="array" ref="C48">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>1.0167999999999999</v>
+      <c r="C48" s="19" cm="1">
+        <f t="array" ref="C48">(Table5[b]/1000*Table4[[#This Row],[li,ges in m]]) + Table5[a]/1000</f>
+        <v>1.0168E-3</v>
       </c>
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
@@ -4153,9 +4150,9 @@
         <f t="shared" si="1"/>
         <v>0.94200000000000006</v>
       </c>
-      <c r="C49" s="14" cm="1">
-        <f t="array" ref="C49">(Table5[b]*Table4[[#This Row],[li,ges in m]]) + Table5[a]</f>
-        <v>0.9768</v>
+      <c r="C49" s="19" cm="1">
+        <f t="array" ref="C49">(Table5[b]/1000*Table4[[#This Row],[li,ges in m]]) + Table5[a]/1000</f>
+        <v>9.7679999999999989E-4</v>
       </c>
       <c r="D49" s="14"/>
       <c r="E49" s="14"/>
@@ -4188,8 +4185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71FA1135-DD52-3C46-BAEB-583B68230B7C}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4245,7 +4242,7 @@
     </row>
     <row r="8" spans="1:7" s="13" customFormat="1" ht="16">
       <c r="A8" s="13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>